<commit_message>
REST API coverage update
Signed-off-by: David Noble <dnoble@splunk.com>
</commit_message>
<xml_diff>
--- a/REST API coverage.xlsx
+++ b/REST API coverage.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="376">
   <si>
     <t>Access Control</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Delete the identified credentials</t>
   </si>
   <si>
-    <t>curl verified : Equivalent to GET authorization/capabilities : no other name but capabilities is permitted</t>
-  </si>
-  <si>
     <t>Applications</t>
   </si>
   <si>
@@ -1069,6 +1066,87 @@
   </si>
   <si>
     <t>Returns the results of the search specified by {search_id}.</t>
+  </si>
+  <si>
+    <t>GET messages</t>
+  </si>
+  <si>
+    <t>Enumerate all systemwide messages.</t>
+  </si>
+  <si>
+    <t>POST messages</t>
+  </si>
+  <si>
+    <t>Create a persistent message displayed at /services/messages.</t>
+  </si>
+  <si>
+    <t>DELETE messages/{name}</t>
+  </si>
+  <si>
+    <t>Deletes a message identified by {name}.</t>
+  </si>
+  <si>
+    <t>GET server/control</t>
+  </si>
+  <si>
+    <t>Lists the actions that can be performed at this endpoint.</t>
+  </si>
+  <si>
+    <t>POST server/control/restart</t>
+  </si>
+  <si>
+    <t>Restarts the Splunk server.</t>
+  </si>
+  <si>
+    <t>GET server/info</t>
+  </si>
+  <si>
+    <t>Enumerates information about the running splunkd.</t>
+  </si>
+  <si>
+    <t>GET server/info/{name}</t>
+  </si>
+  <si>
+    <t>Provides the identical information as /services/server/info. The only valid {name} here is server-info.</t>
+  </si>
+  <si>
+    <t>Redundant with GET server/info</t>
+  </si>
+  <si>
+    <t>GET server/logger</t>
+  </si>
+  <si>
+    <t>Enumerates all splunkd logging categories, either specified in code or in $SPLUNK_HOME/etc/log.cfg.</t>
+  </si>
+  <si>
+    <t>GET server/logger/{name}</t>
+  </si>
+  <si>
+    <t>Describes a specific splunkd logging category.</t>
+  </si>
+  <si>
+    <t>Sets the logging level for a specific logging category.</t>
+  </si>
+  <si>
+    <t>POST server/logger/{name}</t>
+  </si>
+  <si>
+    <t>Splunk.Management</t>
+  </si>
+  <si>
+    <t>1 = Must have in splunk-sdk-csharp-2.0.0</t>
+  </si>
+  <si>
+    <t>2 = Nice to have in splunk-sdk-csharp-2.0.0</t>
+  </si>
+  <si>
+    <t>4 = Redundant endpoint that we will not support</t>
+  </si>
+  <si>
+    <t>Redundant with GET authorization/capabilities</t>
+  </si>
+  <si>
+    <t>3 = Splunk management API, perhaps code named splunk-management-1.0.0 that I'll argue should be the heart of a set of Windows PowerShell commands for managing Splunk servers</t>
   </si>
 </sst>
 </file>
@@ -1207,8 +1285,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E178" totalsRowShown="0">
-  <autoFilter ref="A1:E178"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E187" totalsRowShown="0">
+  <autoFilter ref="A1:E187"/>
   <sortState ref="A2:E178">
     <sortCondition ref="D1:D178"/>
   </sortState>
@@ -1545,15 +1623,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E178"/>
+  <dimension ref="A1:E209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="54.33203125" customWidth="1"/>
+    <col min="1" max="1" width="59.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="106.5" customWidth="1"/>
     <col min="3" max="3" width="8.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
@@ -1579,10 +1657,10 @@
     </row>
     <row r="2" spans="1:5" outlineLevel="1">
       <c r="A2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="D2" s="19">
         <v>1</v>
@@ -1591,10 +1669,10 @@
     </row>
     <row r="3" spans="1:5" outlineLevel="1">
       <c r="A3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
         <v>80</v>
-      </c>
-      <c r="B3" t="s">
-        <v>81</v>
       </c>
       <c r="D3" s="19">
         <v>1</v>
@@ -1603,10 +1681,10 @@
     </row>
     <row r="4" spans="1:5" outlineLevel="1">
       <c r="A4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
       </c>
       <c r="D4" s="19">
         <v>1</v>
@@ -1615,10 +1693,10 @@
     </row>
     <row r="5" spans="1:5" outlineLevel="1">
       <c r="A5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
         <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>85</v>
       </c>
       <c r="D5" s="19">
         <v>1</v>
@@ -1627,10 +1705,10 @@
     </row>
     <row r="6" spans="1:5" outlineLevel="1">
       <c r="A6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
         <v>86</v>
-      </c>
-      <c r="B6" t="s">
-        <v>87</v>
       </c>
       <c r="D6" s="19">
         <v>1</v>
@@ -1639,10 +1717,10 @@
     </row>
     <row r="7" spans="1:5" outlineLevel="1">
       <c r="A7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
         <v>88</v>
-      </c>
-      <c r="B7" t="s">
-        <v>89</v>
       </c>
       <c r="D7" s="19">
         <v>1</v>
@@ -1651,10 +1729,10 @@
     </row>
     <row r="8" spans="1:5" outlineLevel="1">
       <c r="A8" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
         <v>102</v>
-      </c>
-      <c r="B8" t="s">
-        <v>103</v>
       </c>
       <c r="D8" s="19">
         <v>1</v>
@@ -1663,10 +1741,10 @@
     </row>
     <row r="9" spans="1:5" outlineLevel="1">
       <c r="A9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" t="s">
         <v>90</v>
-      </c>
-      <c r="B9" t="s">
-        <v>91</v>
       </c>
       <c r="D9" s="19">
         <v>1</v>
@@ -1675,10 +1753,10 @@
     </row>
     <row r="10" spans="1:5" outlineLevel="1">
       <c r="A10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
         <v>92</v>
-      </c>
-      <c r="B10" t="s">
-        <v>93</v>
       </c>
       <c r="D10" s="19">
         <v>1</v>
@@ -1687,10 +1765,10 @@
     </row>
     <row r="11" spans="1:5" outlineLevel="1">
       <c r="A11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s">
         <v>94</v>
-      </c>
-      <c r="B11" t="s">
-        <v>95</v>
       </c>
       <c r="D11" s="19">
         <v>1</v>
@@ -1699,10 +1777,10 @@
     </row>
     <row r="12" spans="1:5" outlineLevel="1">
       <c r="A12" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="23">
@@ -1712,10 +1790,10 @@
     </row>
     <row r="13" spans="1:5" outlineLevel="1">
       <c r="A13" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="23">
@@ -1725,10 +1803,10 @@
     </row>
     <row r="14" spans="1:5" outlineLevel="1">
       <c r="A14" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="23">
@@ -1738,10 +1816,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>76</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>77</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="23">
@@ -1749,186 +1827,186 @@
       </c>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="16" spans="1:5" outlineLevel="1">
       <c r="A16" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" t="s">
         <v>128</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" s="19">
+        <v>1</v>
+      </c>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5" outlineLevel="1">
+      <c r="A17" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D16" s="19">
-        <v>1</v>
-      </c>
-      <c r="E16" s="20"/>
-    </row>
-    <row r="17" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A17" s="4" t="s">
+      <c r="B17" t="s">
         <v>130</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" s="19">
+        <v>1</v>
+      </c>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" outlineLevel="1">
+      <c r="A18" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="19">
-        <v>1</v>
-      </c>
-      <c r="E17" s="20"/>
-    </row>
-    <row r="18" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A18" s="4" t="s">
+      <c r="B18" t="s">
         <v>132</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" s="19">
+        <v>1</v>
+      </c>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5" outlineLevel="1">
+      <c r="A19" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="D18" s="19">
-        <v>1</v>
-      </c>
-      <c r="E18" s="20"/>
-    </row>
-    <row r="19" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A19" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="22"/>
     </row>
-    <row r="20" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="20" spans="1:5" outlineLevel="1">
       <c r="A20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" t="s">
         <v>136</v>
-      </c>
-      <c r="B20" t="s">
-        <v>137</v>
       </c>
       <c r="D20" s="19">
         <v>2</v>
       </c>
       <c r="E20" s="20"/>
     </row>
-    <row r="21" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="21" spans="1:5" outlineLevel="1">
       <c r="A21" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="22"/>
     </row>
-    <row r="22" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="22" spans="1:5" outlineLevel="1">
       <c r="A22" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" t="s">
         <v>140</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" s="23">
+        <v>1</v>
+      </c>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
+      <c r="A23" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="D22" s="19">
-        <v>2</v>
-      </c>
-      <c r="E22" s="20"/>
-    </row>
-    <row r="23" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
-      <c r="A23" s="18" t="s">
+      <c r="B23" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="24" spans="1:5" outlineLevel="1">
       <c r="A24" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B24" t="s">
         <v>144</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" s="23">
+        <v>1</v>
+      </c>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5" outlineLevel="1">
+      <c r="A25" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D24" s="19">
-        <v>2</v>
-      </c>
-      <c r="E24" s="20"/>
-    </row>
-    <row r="25" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A25" s="4" t="s">
+      <c r="B25" t="s">
         <v>146</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" s="23">
+        <v>1</v>
+      </c>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="1:5" outlineLevel="1">
+      <c r="A26" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D25" s="19">
-        <v>2</v>
-      </c>
-      <c r="E25" s="20"/>
-    </row>
-    <row r="26" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="D26" s="23">
+        <v>1</v>
+      </c>
+      <c r="E26" s="20"/>
+    </row>
+    <row r="27" spans="1:5" outlineLevel="1">
+      <c r="A27" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="D26" s="19">
-        <v>2</v>
-      </c>
-      <c r="E26" s="20"/>
-    </row>
-    <row r="27" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A27" s="4" t="s">
+      <c r="B27" t="s">
         <v>150</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="23">
+        <v>1</v>
+      </c>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5" outlineLevel="1">
+      <c r="A28" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" t="s">
         <v>151</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="19">
-        <v>1</v>
-      </c>
-      <c r="E27" s="20"/>
-    </row>
-    <row r="28" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A28" s="4" t="s">
+      <c r="D28" s="23">
+        <v>1</v>
+      </c>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5" outlineLevel="1">
+      <c r="A29" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B28" t="s">
-        <v>152</v>
-      </c>
-      <c r="D28" s="19">
-        <v>1</v>
-      </c>
-      <c r="E28" s="20"/>
-    </row>
-    <row r="29" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A29" s="4" t="s">
+      <c r="B29" t="s">
         <v>154</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" s="23">
+        <v>1</v>
+      </c>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="1:5" outlineLevel="1">
+      <c r="A30" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="D29" s="19">
-        <v>1</v>
-      </c>
-      <c r="E29" s="20"/>
-    </row>
-    <row r="30" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A30" s="18" t="s">
+      <c r="B30" s="11" t="s">
         <v>156</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>157</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="23">
@@ -1936,12 +2014,12 @@
       </c>
       <c r="E30" s="22"/>
     </row>
-    <row r="31" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="31" spans="1:5" outlineLevel="1">
       <c r="A31" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="23">
@@ -1949,113 +2027,113 @@
       </c>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="32" spans="1:5" outlineLevel="1">
       <c r="A32" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" t="s">
         <v>160</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" s="19">
+        <v>3</v>
+      </c>
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" spans="1:5" outlineLevel="1">
+      <c r="A33" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D32" s="19">
-        <v>2</v>
-      </c>
-      <c r="E32" s="20"/>
-    </row>
-    <row r="33" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A33" s="4" t="s">
+      <c r="B33" t="s">
         <v>162</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" s="19">
+        <v>3</v>
+      </c>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="1:5" outlineLevel="1">
+      <c r="A34" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="19">
-        <v>2</v>
-      </c>
-      <c r="E33" s="20"/>
-    </row>
-    <row r="34" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A34" s="4" t="s">
+      <c r="B34" t="s">
         <v>164</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" s="19">
+        <v>3</v>
+      </c>
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
+      <c r="A35" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D34" s="19">
-        <v>2</v>
-      </c>
-      <c r="E34" s="20"/>
-    </row>
-    <row r="35" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
-      <c r="A35" s="4" t="s">
+      <c r="B35" t="s">
         <v>166</v>
-      </c>
-      <c r="B35" t="s">
-        <v>167</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E35" s="20"/>
     </row>
-    <row r="36" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="36" spans="1:5" outlineLevel="1">
       <c r="A36" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="C36" s="12"/>
+      <c r="D36" s="19">
+        <v>3</v>
+      </c>
+      <c r="E36" s="22"/>
+    </row>
+    <row r="37" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
+      <c r="A37" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="23">
-        <v>1</v>
-      </c>
-      <c r="E36" s="22"/>
-    </row>
-    <row r="37" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
-      <c r="A37" s="4" t="s">
+      <c r="B37" t="s">
         <v>170</v>
-      </c>
-      <c r="B37" t="s">
-        <v>171</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E37" s="20"/>
     </row>
-    <row r="38" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="38" spans="1:5" outlineLevel="1">
       <c r="A38" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="C38" s="12"/>
+      <c r="D38" s="19">
+        <v>3</v>
+      </c>
+      <c r="E38" s="22"/>
+    </row>
+    <row r="39" spans="1:5" outlineLevel="1">
+      <c r="A39" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="23">
-        <v>2</v>
-      </c>
-      <c r="E38" s="22"/>
-    </row>
-    <row r="39" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A39" s="18" t="s">
+      <c r="B39" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="C39" s="12"/>
+      <c r="D39" s="19">
+        <v>3</v>
+      </c>
+      <c r="E39" s="22"/>
+    </row>
+    <row r="40" spans="1:5" outlineLevel="1">
+      <c r="A40" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="23">
-        <v>2</v>
-      </c>
-      <c r="E39" s="22"/>
-    </row>
-    <row r="40" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A40" s="18" t="s">
+      <c r="B40" s="11" t="s">
         <v>176</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>177</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="23">
@@ -2063,42 +2141,42 @@
       </c>
       <c r="E40" s="22"/>
     </row>
-    <row r="41" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="41" spans="1:5" outlineLevel="1">
       <c r="A41" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="C41" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="23">
+        <v>1</v>
+      </c>
+      <c r="E41" s="22"/>
+    </row>
+    <row r="42" spans="1:5" outlineLevel="1">
+      <c r="A42" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="C41" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="23">
-        <v>1</v>
-      </c>
-      <c r="E41" s="22"/>
-    </row>
-    <row r="42" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A42" s="18" t="s">
+      <c r="B42" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="C42" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="23">
+        <v>1</v>
+      </c>
+      <c r="E42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" outlineLevel="1">
+      <c r="A43" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C42" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="23">
-        <v>1</v>
-      </c>
-      <c r="E42" s="22"/>
-    </row>
-    <row r="43" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A43" s="18" t="s">
+      <c r="B43" s="11" t="s">
         <v>182</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>183</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="23">
@@ -2106,27 +2184,27 @@
       </c>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="44" spans="1:5" outlineLevel="1">
       <c r="A44" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="C44" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="23">
+        <v>1</v>
+      </c>
+      <c r="E44" s="22"/>
+    </row>
+    <row r="45" spans="1:5" outlineLevel="1">
+      <c r="A45" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="23">
-        <v>1</v>
-      </c>
-      <c r="E44" s="22"/>
-    </row>
-    <row r="45" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A45" s="18" t="s">
+      <c r="B45" s="11" t="s">
         <v>186</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>187</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="23">
@@ -2134,72 +2212,72 @@
       </c>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="46" spans="1:5" outlineLevel="1">
       <c r="A46" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="C46" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="23">
+        <v>1</v>
+      </c>
+      <c r="E46" s="22"/>
+    </row>
+    <row r="47" spans="1:5" outlineLevel="1">
+      <c r="A47" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" s="23">
-        <v>1</v>
-      </c>
-      <c r="E46" s="22"/>
-    </row>
-    <row r="47" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A47" s="18" t="s">
+      <c r="B47" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="23">
+        <v>1</v>
+      </c>
+      <c r="E47" s="22"/>
+    </row>
+    <row r="48" spans="1:5" outlineLevel="1">
+      <c r="A48" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B48" s="11" t="s">
         <v>348</v>
       </c>
-      <c r="C47" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="23">
-        <v>1</v>
-      </c>
-      <c r="E47" s="22"/>
-    </row>
-    <row r="48" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A48" s="18" t="s">
+      <c r="C48" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48" s="23">
+        <v>1</v>
+      </c>
+      <c r="E48" s="22"/>
+    </row>
+    <row r="49" spans="1:5" outlineLevel="1">
+      <c r="A49" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>349</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="23">
-        <v>1</v>
-      </c>
-      <c r="E48" s="22"/>
-    </row>
-    <row r="49" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A49" s="18" t="s">
+      <c r="B49" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="C49" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" s="23">
+        <v>1</v>
+      </c>
+      <c r="E49" s="22"/>
+    </row>
+    <row r="50" spans="1:5" outlineLevel="1">
+      <c r="A50" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="23">
-        <v>1</v>
-      </c>
-      <c r="E49" s="22"/>
-    </row>
-    <row r="50" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A50" s="18" t="s">
+      <c r="B50" s="11" t="s">
         <v>194</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>195</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="23">
@@ -2207,38 +2285,38 @@
       </c>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="51" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
       <c r="A51" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>196</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>197</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="52" spans="1:5" outlineLevel="1">
       <c r="A52" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B52" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52" s="22"/>
     </row>
-    <row r="53" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="53" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
       <c r="A53" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B53" t="s">
         <v>200</v>
-      </c>
-      <c r="B53" t="s">
-        <v>201</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="19">
@@ -2246,12 +2324,12 @@
       </c>
       <c r="E53" s="20"/>
     </row>
-    <row r="54" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="54" spans="1:5" outlineLevel="1">
       <c r="A54" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B54" s="11" t="s">
         <v>202</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="23">
@@ -2259,12 +2337,12 @@
       </c>
       <c r="E54" s="22"/>
     </row>
-    <row r="55" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="55" spans="1:5" outlineLevel="1">
       <c r="A55" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>205</v>
       </c>
       <c r="C55" s="12"/>
       <c r="D55" s="23">
@@ -2272,22 +2350,22 @@
       </c>
       <c r="E55" s="22"/>
     </row>
-    <row r="56" spans="1:5" collapsed="1">
+    <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B56" s="20" t="s">
-        <v>127</v>
-      </c>
       <c r="C56" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D56" s="19">
         <v>1</v>
       </c>
       <c r="E56" s="20"/>
     </row>
-    <row r="57" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="57" spans="1:5" outlineLevel="1">
       <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
@@ -2302,7 +2380,7 @@
       </c>
       <c r="E57" s="20"/>
     </row>
-    <row r="58" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="58" spans="1:5" outlineLevel="1">
       <c r="A58" s="4" t="s">
         <v>6</v>
       </c>
@@ -2314,7 +2392,7 @@
       </c>
       <c r="E58" s="20"/>
     </row>
-    <row r="59" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="59" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
       <c r="A59" s="4" t="s">
         <v>10</v>
       </c>
@@ -2329,7 +2407,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="60" spans="1:5" outlineLevel="1">
       <c r="A60" s="4" t="s">
         <v>15</v>
       </c>
@@ -2341,7 +2419,7 @@
       </c>
       <c r="E60" s="20"/>
     </row>
-    <row r="61" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="61" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
       <c r="A61" s="4" t="s">
         <v>16</v>
       </c>
@@ -2356,7 +2434,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="62" spans="1:5" outlineLevel="1">
       <c r="A62" s="4" t="s">
         <v>20</v>
       </c>
@@ -2368,7 +2446,7 @@
       </c>
       <c r="E62" s="20"/>
     </row>
-    <row r="63" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="63" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
       <c r="A63" s="4" t="s">
         <v>19</v>
       </c>
@@ -2381,7 +2459,7 @@
       </c>
       <c r="E63" s="20"/>
     </row>
-    <row r="64" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="64" spans="1:5" outlineLevel="1">
       <c r="A64" s="4" t="s">
         <v>25</v>
       </c>
@@ -2393,7 +2471,7 @@
       </c>
       <c r="E64" s="20"/>
     </row>
-    <row r="65" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="65" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
       <c r="A65" s="4" t="s">
         <v>26</v>
       </c>
@@ -2406,7 +2484,7 @@
       </c>
       <c r="E65" s="20"/>
     </row>
-    <row r="66" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="66" spans="1:5" outlineLevel="1">
       <c r="A66" s="4" t="s">
         <v>27</v>
       </c>
@@ -2418,7 +2496,7 @@
       </c>
       <c r="E66" s="20"/>
     </row>
-    <row r="67" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="67" spans="1:5" s="10" customFormat="1" outlineLevel="1" collapsed="1">
       <c r="A67" s="4" t="s">
         <v>23</v>
       </c>
@@ -2431,7 +2509,7 @@
       </c>
       <c r="E67" s="20"/>
     </row>
-    <row r="68" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="68" spans="1:5" outlineLevel="1">
       <c r="A68" s="4" t="s">
         <v>31</v>
       </c>
@@ -2439,11 +2517,11 @@
         <v>32</v>
       </c>
       <c r="D68" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E68" s="20"/>
     </row>
-    <row r="69" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="69" spans="1:5" outlineLevel="1">
       <c r="A69" s="4" t="s">
         <v>33</v>
       </c>
@@ -2451,13 +2529,13 @@
         <v>34</v>
       </c>
       <c r="D69" s="19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E69" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" hidden="1" outlineLevel="1">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" outlineLevel="1">
       <c r="A70" s="4" t="s">
         <v>35</v>
       </c>
@@ -2469,7 +2547,7 @@
       </c>
       <c r="E70" s="20"/>
     </row>
-    <row r="71" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="71" spans="1:5" outlineLevel="1">
       <c r="A71" s="4" t="s">
         <v>36</v>
       </c>
@@ -2481,7 +2559,7 @@
       </c>
       <c r="E71" s="20"/>
     </row>
-    <row r="72" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="72" spans="1:5" outlineLevel="1">
       <c r="A72" s="4" t="s">
         <v>39</v>
       </c>
@@ -2493,7 +2571,7 @@
       </c>
       <c r="E72" s="20"/>
     </row>
-    <row r="73" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="73" spans="1:5" outlineLevel="1">
       <c r="A73" s="4" t="s">
         <v>40</v>
       </c>
@@ -2505,7 +2583,7 @@
       </c>
       <c r="E73" s="20"/>
     </row>
-    <row r="74" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="74" spans="1:5" outlineLevel="1">
       <c r="A74" s="4" t="s">
         <v>41</v>
       </c>
@@ -2517,7 +2595,7 @@
       </c>
       <c r="E74" s="20"/>
     </row>
-    <row r="75" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="75" spans="1:5" outlineLevel="1">
       <c r="A75" s="4" t="s">
         <v>45</v>
       </c>
@@ -2525,11 +2603,11 @@
         <v>46</v>
       </c>
       <c r="D75" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E75" s="20"/>
     </row>
-    <row r="76" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="76" spans="1:5" outlineLevel="1">
       <c r="A76" s="4" t="s">
         <v>47</v>
       </c>
@@ -2537,11 +2615,11 @@
         <v>48</v>
       </c>
       <c r="D76" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E76" s="20"/>
     </row>
-    <row r="77" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="77" spans="1:5" outlineLevel="1">
       <c r="A77" s="4" t="s">
         <v>49</v>
       </c>
@@ -2549,93 +2627,93 @@
         <v>50</v>
       </c>
       <c r="D77" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E77" s="20"/>
     </row>
-    <row r="78" spans="1:5" collapsed="1">
+    <row r="78" spans="1:5">
       <c r="A78" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D78" s="19">
         <v>1</v>
       </c>
       <c r="E78" s="20"/>
     </row>
-    <row r="79" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="79" spans="1:5" outlineLevel="1">
       <c r="A79" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B79" t="s">
+        <v>107</v>
+      </c>
+      <c r="D79" s="19">
+        <v>1</v>
+      </c>
+      <c r="E79" s="20"/>
+    </row>
+    <row r="80" spans="1:5" outlineLevel="1">
+      <c r="A80" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="B79" t="s">
-        <v>108</v>
-      </c>
-      <c r="D79" s="19">
-        <v>2</v>
-      </c>
-      <c r="E79" s="20"/>
-    </row>
-    <row r="80" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A80" s="18" t="s">
+      <c r="B80" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="C80" s="12"/>
+      <c r="D80" s="19">
+        <v>1</v>
+      </c>
+      <c r="E80" s="22"/>
+    </row>
+    <row r="81" spans="1:5" outlineLevel="1">
+      <c r="A81" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="23">
-        <v>2</v>
-      </c>
-      <c r="E80" s="22"/>
-    </row>
-    <row r="81" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A81" s="18" t="s">
+      <c r="B81" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="C81" s="12"/>
+      <c r="D81" s="19">
+        <v>1</v>
+      </c>
+      <c r="E81" s="22"/>
+    </row>
+    <row r="82" spans="1:5" outlineLevel="1">
+      <c r="A82" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C81" s="12"/>
-      <c r="D81" s="23">
-        <v>2</v>
-      </c>
-      <c r="E81" s="22"/>
-    </row>
-    <row r="82" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A82" s="4" t="s">
+      <c r="B82" t="s">
         <v>114</v>
       </c>
-      <c r="B82" t="s">
+      <c r="D82" s="19">
+        <v>1</v>
+      </c>
+      <c r="E82" s="20"/>
+    </row>
+    <row r="83" spans="1:5" outlineLevel="1">
+      <c r="A83" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D82" s="19">
-        <v>2</v>
-      </c>
-      <c r="E82" s="20"/>
-    </row>
-    <row r="83" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A83" s="4" t="s">
+      <c r="B83" t="s">
         <v>116</v>
       </c>
-      <c r="B83" t="s">
-        <v>117</v>
-      </c>
       <c r="D83" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E83" s="20"/>
     </row>
-    <row r="84" spans="1:5" collapsed="1">
+    <row r="84" spans="1:5">
       <c r="A84" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B84" s="20" t="s">
         <v>106</v>
-      </c>
-      <c r="B84" s="20" t="s">
-        <v>107</v>
       </c>
       <c r="C84" s="9"/>
       <c r="D84" s="19">
@@ -2643,774 +2721,910 @@
       </c>
       <c r="E84" s="20"/>
     </row>
-    <row r="85" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="85" spans="1:5" outlineLevel="1">
       <c r="A85" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B85" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="B85" s="20" t="s">
+      <c r="C85" s="9"/>
+      <c r="D85" s="19">
+        <v>3</v>
+      </c>
+      <c r="E85" s="20"/>
+    </row>
+    <row r="86" spans="1:5" outlineLevel="1">
+      <c r="A86" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="C85" s="9"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="20"/>
-    </row>
-    <row r="86" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A86" s="4" t="s">
+      <c r="B86" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="B86" s="20" t="s">
-        <v>346</v>
-      </c>
       <c r="C86" s="9"/>
-      <c r="D86" s="19"/>
+      <c r="D86" s="19">
+        <v>3</v>
+      </c>
       <c r="E86" s="20"/>
     </row>
-    <row r="87" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="87" spans="1:5" outlineLevel="1">
       <c r="A87" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B87" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="B87" s="20" t="s">
+      <c r="C87" s="9"/>
+      <c r="D87" s="19">
+        <v>3</v>
+      </c>
+      <c r="E87" s="20"/>
+    </row>
+    <row r="88" spans="1:5" outlineLevel="1">
+      <c r="A88" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="C87" s="9"/>
-      <c r="D87" s="19"/>
-      <c r="E87" s="20"/>
-    </row>
-    <row r="88" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A88" s="4" t="s">
+      <c r="B88" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="C88" s="9"/>
+      <c r="D88" s="19">
+        <v>3</v>
+      </c>
+      <c r="E88" s="20"/>
+    </row>
+    <row r="89" spans="1:5" outlineLevel="1">
+      <c r="A89" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C88" s="9"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="20"/>
-    </row>
-    <row r="89" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A89" s="4" t="s">
+      <c r="B89" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="B89" s="20" t="s">
-        <v>342</v>
-      </c>
       <c r="C89" s="9"/>
-      <c r="D89" s="19"/>
+      <c r="D89" s="19">
+        <v>3</v>
+      </c>
       <c r="E89" s="20"/>
     </row>
-    <row r="90" spans="1:5" hidden="1" outlineLevel="1" collapsed="1">
+    <row r="90" spans="1:5" outlineLevel="1" collapsed="1">
       <c r="A90" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B90" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="B90" s="20" t="s">
-        <v>336</v>
-      </c>
       <c r="C90" s="9"/>
-      <c r="D90" s="19"/>
+      <c r="D90" s="19">
+        <v>3</v>
+      </c>
       <c r="E90" s="20"/>
     </row>
-    <row r="91" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="91" spans="1:5" outlineLevel="1">
       <c r="A91" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B91" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="B91" s="20" t="s">
-        <v>334</v>
-      </c>
       <c r="C91" s="9"/>
-      <c r="D91" s="19"/>
+      <c r="D91" s="19">
+        <v>3</v>
+      </c>
       <c r="E91" s="20"/>
     </row>
-    <row r="92" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="92" spans="1:5" outlineLevel="1">
       <c r="A92" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B92" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="B92" s="20" t="s">
+      <c r="C92" s="9"/>
+      <c r="D92" s="19">
+        <v>3</v>
+      </c>
+      <c r="E92" s="20"/>
+    </row>
+    <row r="93" spans="1:5" outlineLevel="1">
+      <c r="A93" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="C92" s="9"/>
-      <c r="D92" s="19"/>
-      <c r="E92" s="20"/>
-    </row>
-    <row r="93" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A93" s="4" t="s">
+      <c r="B93" s="20" t="s">
         <v>331</v>
       </c>
-      <c r="B93" s="20" t="s">
-        <v>332</v>
-      </c>
       <c r="C93" s="9"/>
-      <c r="D93" s="19"/>
+      <c r="D93" s="19">
+        <v>3</v>
+      </c>
       <c r="E93" s="20"/>
     </row>
-    <row r="94" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="94" spans="1:5" outlineLevel="1">
       <c r="A94" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="B94" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="B94" s="20" t="s">
+      <c r="C94" s="9"/>
+      <c r="D94" s="19">
+        <v>3</v>
+      </c>
+      <c r="E94" s="20"/>
+    </row>
+    <row r="95" spans="1:5" outlineLevel="1">
+      <c r="A95" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="C94" s="9"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="20"/>
-    </row>
-    <row r="95" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A95" s="4" t="s">
+      <c r="B95" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="B95" s="20" t="s">
+      <c r="C95" s="9"/>
+      <c r="D95" s="19">
+        <v>3</v>
+      </c>
+      <c r="E95" s="20"/>
+    </row>
+    <row r="96" spans="1:5" outlineLevel="1" collapsed="1">
+      <c r="A96" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="C95" s="9"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="20"/>
-    </row>
-    <row r="96" spans="1:5" hidden="1" outlineLevel="1" collapsed="1">
-      <c r="A96" s="4" t="s">
+      <c r="B96" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="B96" s="20" t="s">
-        <v>328</v>
-      </c>
       <c r="C96" s="9"/>
-      <c r="D96" s="19"/>
+      <c r="D96" s="19">
+        <v>3</v>
+      </c>
       <c r="E96" s="20"/>
     </row>
-    <row r="97" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="97" spans="1:5" outlineLevel="1">
       <c r="A97" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B97" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="B97" s="20" t="s">
-        <v>322</v>
-      </c>
       <c r="C97" s="9"/>
-      <c r="D97" s="19"/>
+      <c r="D97" s="19">
+        <v>3</v>
+      </c>
       <c r="E97" s="20"/>
     </row>
-    <row r="98" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="98" spans="1:5" outlineLevel="1">
       <c r="A98" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B98" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="B98" s="20" t="s">
+      <c r="C98" s="9"/>
+      <c r="D98" s="19">
+        <v>3</v>
+      </c>
+      <c r="E98" s="20"/>
+    </row>
+    <row r="99" spans="1:5" outlineLevel="1">
+      <c r="A99" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="C98" s="9"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="20"/>
-    </row>
-    <row r="99" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A99" s="4" t="s">
+      <c r="B99" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="B99" s="20" t="s">
-        <v>320</v>
-      </c>
       <c r="C99" s="9"/>
-      <c r="D99" s="19"/>
+      <c r="D99" s="19">
+        <v>3</v>
+      </c>
       <c r="E99" s="20"/>
     </row>
-    <row r="100" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="100" spans="1:5" outlineLevel="1">
       <c r="A100" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B100" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="B100" s="20" t="s">
-        <v>316</v>
-      </c>
       <c r="C100" s="9"/>
-      <c r="D100" s="19"/>
+      <c r="D100" s="19">
+        <v>3</v>
+      </c>
       <c r="E100" s="20"/>
     </row>
-    <row r="101" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="101" spans="1:5" outlineLevel="1">
       <c r="A101" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B101" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="B101" s="20" t="s">
-        <v>314</v>
-      </c>
       <c r="C101" s="9"/>
-      <c r="D101" s="19"/>
+      <c r="D101" s="19">
+        <v>3</v>
+      </c>
       <c r="E101" s="20"/>
     </row>
-    <row r="102" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="102" spans="1:5" outlineLevel="1">
       <c r="A102" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B102" s="20" t="s">
         <v>311</v>
       </c>
-      <c r="B102" s="20" t="s">
+      <c r="C102" s="9"/>
+      <c r="D102" s="19">
+        <v>3</v>
+      </c>
+      <c r="E102" s="20"/>
+    </row>
+    <row r="103" spans="1:5" outlineLevel="1">
+      <c r="A103" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="C102" s="9"/>
-      <c r="D102" s="19"/>
-      <c r="E102" s="20"/>
-    </row>
-    <row r="103" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A103" s="4" t="s">
+      <c r="B103" s="20" t="s">
         <v>313</v>
       </c>
-      <c r="B103" s="20" t="s">
-        <v>314</v>
-      </c>
       <c r="C103" s="9"/>
-      <c r="D103" s="19"/>
+      <c r="D103" s="19">
+        <v>3</v>
+      </c>
       <c r="E103" s="20"/>
     </row>
-    <row r="104" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="104" spans="1:5" outlineLevel="1">
       <c r="A104" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B104" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="B104" s="20" t="s">
+      <c r="C104" s="9"/>
+      <c r="D104" s="19">
+        <v>3</v>
+      </c>
+      <c r="E104" s="20"/>
+    </row>
+    <row r="105" spans="1:5" outlineLevel="1">
+      <c r="A105" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C104" s="9"/>
-      <c r="D104" s="19"/>
-      <c r="E104" s="20"/>
-    </row>
-    <row r="105" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A105" s="4" t="s">
+      <c r="B105" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="B105" s="20" t="s">
+      <c r="C105" s="9"/>
+      <c r="D105" s="19">
+        <v>3</v>
+      </c>
+      <c r="E105" s="20"/>
+    </row>
+    <row r="106" spans="1:5" outlineLevel="1">
+      <c r="A106" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="C105" s="9"/>
-      <c r="D105" s="19"/>
-      <c r="E105" s="20"/>
-    </row>
-    <row r="106" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A106" s="4" t="s">
+      <c r="B106" s="20" t="s">
         <v>309</v>
       </c>
-      <c r="B106" s="20" t="s">
-        <v>310</v>
-      </c>
       <c r="C106" s="9"/>
-      <c r="D106" s="19"/>
+      <c r="D106" s="19">
+        <v>3</v>
+      </c>
       <c r="E106" s="20"/>
     </row>
-    <row r="107" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="107" spans="1:5" outlineLevel="1">
       <c r="A107" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B107" s="20" t="s">
         <v>301</v>
       </c>
-      <c r="B107" s="20" t="s">
+      <c r="C107" s="9"/>
+      <c r="D107" s="19">
+        <v>3</v>
+      </c>
+      <c r="E107" s="20"/>
+    </row>
+    <row r="108" spans="1:5" outlineLevel="1">
+      <c r="A108" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="C107" s="9"/>
-      <c r="D107" s="19"/>
-      <c r="E107" s="20"/>
-    </row>
-    <row r="108" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A108" s="4" t="s">
+      <c r="B108" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="B108" s="20" t="s">
-        <v>304</v>
-      </c>
       <c r="C108" s="9"/>
-      <c r="D108" s="19"/>
+      <c r="D108" s="19">
+        <v>3</v>
+      </c>
       <c r="E108" s="20"/>
     </row>
-    <row r="109" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="109" spans="1:5" outlineLevel="1">
       <c r="A109" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B109" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="B109" s="20" t="s">
-        <v>300</v>
-      </c>
       <c r="C109" s="9"/>
-      <c r="D109" s="19"/>
+      <c r="D109" s="19">
+        <v>3</v>
+      </c>
       <c r="E109" s="20"/>
     </row>
-    <row r="110" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="110" spans="1:5" outlineLevel="1">
       <c r="A110" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B110" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="C110" s="9"/>
+      <c r="D110" s="19">
+        <v>3</v>
+      </c>
+      <c r="E110" s="20"/>
+    </row>
+    <row r="111" spans="1:5" outlineLevel="1">
+      <c r="A111" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="C110" s="9"/>
-      <c r="D110" s="19"/>
-      <c r="E110" s="20"/>
-    </row>
-    <row r="111" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A111" s="4" t="s">
+      <c r="B111" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="B111" s="20" t="s">
+      <c r="C111" s="9"/>
+      <c r="D111" s="19">
+        <v>3</v>
+      </c>
+      <c r="E111" s="20"/>
+    </row>
+    <row r="112" spans="1:5" outlineLevel="1">
+      <c r="A112" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="C111" s="9"/>
-      <c r="D111" s="19"/>
-      <c r="E111" s="20"/>
-    </row>
-    <row r="112" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A112" s="4" t="s">
+      <c r="B112" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="B112" s="20" t="s">
-        <v>298</v>
-      </c>
       <c r="C112" s="9"/>
-      <c r="D112" s="19"/>
+      <c r="D112" s="19">
+        <v>3</v>
+      </c>
       <c r="E112" s="20"/>
     </row>
-    <row r="113" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="113" spans="1:5" outlineLevel="1">
       <c r="A113" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B113" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="B113" s="20" t="s">
+      <c r="C113" s="9"/>
+      <c r="D113" s="19">
+        <v>3</v>
+      </c>
+      <c r="E113" s="20"/>
+    </row>
+    <row r="114" spans="1:5" outlineLevel="1">
+      <c r="A114" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="C113" s="9"/>
-      <c r="D113" s="19"/>
-      <c r="E113" s="20"/>
-    </row>
-    <row r="114" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A114" s="4" t="s">
+      <c r="B114" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="B114" s="20" t="s">
-        <v>292</v>
-      </c>
       <c r="C114" s="9"/>
-      <c r="D114" s="19"/>
+      <c r="D114" s="19">
+        <v>3</v>
+      </c>
       <c r="E114" s="20"/>
     </row>
-    <row r="115" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="115" spans="1:5" outlineLevel="1">
       <c r="A115" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B115" s="20" t="s">
         <v>283</v>
       </c>
-      <c r="B115" s="20" t="s">
+      <c r="C115" s="9"/>
+      <c r="D115" s="19">
+        <v>3</v>
+      </c>
+      <c r="E115" s="20"/>
+    </row>
+    <row r="116" spans="1:5" s="10" customFormat="1" outlineLevel="1">
+      <c r="A116" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="C115" s="9"/>
-      <c r="D115" s="19"/>
-      <c r="E115" s="20"/>
-    </row>
-    <row r="116" spans="1:5" s="10" customFormat="1" hidden="1" outlineLevel="1">
-      <c r="A116" s="4" t="s">
+      <c r="B116" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="B116" s="20" t="s">
+      <c r="C116" s="9"/>
+      <c r="D116" s="19">
+        <v>3</v>
+      </c>
+      <c r="E116" s="20"/>
+    </row>
+    <row r="117" spans="1:5" outlineLevel="1">
+      <c r="A117" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="C116" s="9"/>
-      <c r="D116" s="19"/>
-      <c r="E116" s="20"/>
-    </row>
-    <row r="117" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A117" s="4" t="s">
+      <c r="B117" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="B117" s="20" t="s">
-        <v>288</v>
-      </c>
       <c r="C117" s="9"/>
-      <c r="D117" s="19"/>
+      <c r="D117" s="19">
+        <v>3</v>
+      </c>
       <c r="E117" s="20"/>
     </row>
-    <row r="118" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="118" spans="1:5" outlineLevel="1">
       <c r="A118" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B118" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="B118" s="20" t="s">
-        <v>282</v>
-      </c>
       <c r="C118" s="9"/>
-      <c r="D118" s="19"/>
+      <c r="D118" s="19">
+        <v>3</v>
+      </c>
       <c r="E118" s="20"/>
     </row>
-    <row r="119" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="119" spans="1:5" outlineLevel="1">
       <c r="A119" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B119" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="B119" s="20" t="s">
+      <c r="C119" s="9"/>
+      <c r="D119" s="19">
+        <v>3</v>
+      </c>
+      <c r="E119" s="20"/>
+    </row>
+    <row r="120" spans="1:5" outlineLevel="1">
+      <c r="A120" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="C119" s="9"/>
-      <c r="D119" s="19"/>
-      <c r="E119" s="20"/>
-    </row>
-    <row r="120" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A120" s="4" t="s">
+      <c r="B120" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="B120" s="20" t="s">
-        <v>280</v>
-      </c>
       <c r="C120" s="9"/>
-      <c r="D120" s="19"/>
+      <c r="D120" s="19">
+        <v>3</v>
+      </c>
       <c r="E120" s="20"/>
     </row>
-    <row r="121" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="121" spans="1:5" outlineLevel="1">
       <c r="A121" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B121" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="B121" s="20" t="s">
+      <c r="C121" s="9"/>
+      <c r="D121" s="19">
+        <v>3</v>
+      </c>
+      <c r="E121" s="20"/>
+    </row>
+    <row r="122" spans="1:5" outlineLevel="1">
+      <c r="A122" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="C121" s="9"/>
-      <c r="D121" s="19"/>
-      <c r="E121" s="20"/>
-    </row>
-    <row r="122" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A122" s="4" t="s">
+      <c r="B122" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="B122" s="20" t="s">
+      <c r="C122" s="9"/>
+      <c r="D122" s="19">
+        <v>3</v>
+      </c>
+      <c r="E122" s="20"/>
+    </row>
+    <row r="123" spans="1:5" outlineLevel="1">
+      <c r="A123" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="C122" s="9"/>
-      <c r="D122" s="19"/>
-      <c r="E122" s="20"/>
-    </row>
-    <row r="123" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A123" s="4" t="s">
+      <c r="B123" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="B123" s="20" t="s">
-        <v>276</v>
-      </c>
       <c r="C123" s="9"/>
-      <c r="D123" s="19"/>
+      <c r="D123" s="19">
+        <v>3</v>
+      </c>
       <c r="E123" s="20"/>
     </row>
-    <row r="124" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="124" spans="1:5" outlineLevel="1">
       <c r="A124" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B124" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="B124" s="20" t="s">
-        <v>270</v>
-      </c>
       <c r="C124" s="9"/>
-      <c r="D124" s="19"/>
+      <c r="D124" s="19">
+        <v>3</v>
+      </c>
       <c r="E124" s="20"/>
     </row>
-    <row r="125" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="125" spans="1:5" outlineLevel="1">
       <c r="A125" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B125" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="B125" s="20" t="s">
-        <v>268</v>
-      </c>
       <c r="C125" s="9"/>
-      <c r="D125" s="19"/>
+      <c r="D125" s="19">
+        <v>3</v>
+      </c>
       <c r="E125" s="20"/>
     </row>
-    <row r="126" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="126" spans="1:5" outlineLevel="1">
       <c r="A126" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B126" s="20" t="s">
         <v>263</v>
       </c>
-      <c r="B126" s="20" t="s">
+      <c r="C126" s="9"/>
+      <c r="D126" s="19">
+        <v>3</v>
+      </c>
+      <c r="E126" s="20"/>
+    </row>
+    <row r="127" spans="1:5" outlineLevel="1">
+      <c r="A127" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="C126" s="9"/>
-      <c r="D126" s="19"/>
-      <c r="E126" s="20"/>
-    </row>
-    <row r="127" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A127" s="4" t="s">
+      <c r="B127" s="20" t="s">
         <v>265</v>
       </c>
-      <c r="B127" s="20" t="s">
-        <v>266</v>
-      </c>
       <c r="C127" s="9"/>
-      <c r="D127" s="19"/>
+      <c r="D127" s="19">
+        <v>3</v>
+      </c>
       <c r="E127" s="20"/>
     </row>
-    <row r="128" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="128" spans="1:5" outlineLevel="1">
       <c r="A128" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B128" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="B128" s="20" t="s">
+      <c r="C128" s="9"/>
+      <c r="D128" s="19">
+        <v>3</v>
+      </c>
+      <c r="E128" s="20"/>
+    </row>
+    <row r="129" spans="1:5" outlineLevel="1">
+      <c r="A129" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="C128" s="9"/>
-      <c r="D128" s="19"/>
-      <c r="E128" s="20"/>
-    </row>
-    <row r="129" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A129" s="4" t="s">
+      <c r="B129" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="B129" s="20" t="s">
-        <v>262</v>
-      </c>
       <c r="C129" s="9"/>
-      <c r="D129" s="19"/>
+      <c r="D129" s="19">
+        <v>3</v>
+      </c>
       <c r="E129" s="20"/>
     </row>
-    <row r="130" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="130" spans="1:5" outlineLevel="1">
       <c r="A130" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B130" s="20" t="s">
         <v>253</v>
       </c>
-      <c r="B130" s="20" t="s">
+      <c r="C130" s="9"/>
+      <c r="D130" s="19">
+        <v>3</v>
+      </c>
+      <c r="E130" s="20"/>
+    </row>
+    <row r="131" spans="1:5" outlineLevel="1">
+      <c r="A131" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C130" s="9"/>
-      <c r="D130" s="19"/>
-      <c r="E130" s="20"/>
-    </row>
-    <row r="131" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A131" s="4" t="s">
+      <c r="B131" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="C131" s="9"/>
+      <c r="D131" s="19">
+        <v>3</v>
+      </c>
+      <c r="E131" s="20"/>
+    </row>
+    <row r="132" spans="1:5" outlineLevel="1">
+      <c r="A132" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="B131" s="20" t="s">
+      <c r="B132" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="C131" s="9"/>
-      <c r="D131" s="19"/>
-      <c r="E131" s="20"/>
-    </row>
-    <row r="132" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A132" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="B132" s="20" t="s">
-        <v>258</v>
-      </c>
       <c r="C132" s="9"/>
-      <c r="D132" s="19"/>
+      <c r="D132" s="19">
+        <v>3</v>
+      </c>
       <c r="E132" s="20"/>
     </row>
-    <row r="133" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="133" spans="1:5" outlineLevel="1">
       <c r="A133" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B133" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="B133" s="20" t="s">
-        <v>252</v>
-      </c>
       <c r="C133" s="9"/>
-      <c r="D133" s="19"/>
+      <c r="D133" s="19">
+        <v>3</v>
+      </c>
       <c r="E133" s="20"/>
     </row>
-    <row r="134" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="134" spans="1:5" outlineLevel="1">
       <c r="A134" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B134" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="B134" s="20" t="s">
+      <c r="C134" s="9"/>
+      <c r="D134" s="19">
+        <v>3</v>
+      </c>
+      <c r="E134" s="20"/>
+    </row>
+    <row r="135" spans="1:5" outlineLevel="1">
+      <c r="A135" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="C134" s="9"/>
-      <c r="D134" s="19"/>
-      <c r="E134" s="20"/>
-    </row>
-    <row r="135" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A135" s="4" t="s">
+      <c r="B135" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C135" s="9"/>
+      <c r="D135" s="19">
+        <v>3</v>
+      </c>
+      <c r="E135" s="20"/>
+    </row>
+    <row r="136" spans="1:5" outlineLevel="1">
+      <c r="A136" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="B135" s="20" t="s">
+      <c r="B136" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="C135" s="9"/>
-      <c r="D135" s="19"/>
-      <c r="E135" s="20"/>
-    </row>
-    <row r="136" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A136" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="B136" s="20" t="s">
-        <v>250</v>
-      </c>
       <c r="C136" s="9"/>
-      <c r="D136" s="19"/>
+      <c r="D136" s="19">
+        <v>3</v>
+      </c>
       <c r="E136" s="20"/>
     </row>
-    <row r="137" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="137" spans="1:5" outlineLevel="1">
       <c r="A137" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B137" s="20" t="s">
         <v>241</v>
       </c>
-      <c r="B137" s="20" t="s">
+      <c r="C137" s="9"/>
+      <c r="D137" s="19">
+        <v>3</v>
+      </c>
+      <c r="E137" s="20"/>
+    </row>
+    <row r="138" spans="1:5" outlineLevel="1">
+      <c r="A138" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C137" s="9"/>
-      <c r="D137" s="19"/>
-      <c r="E137" s="20"/>
-    </row>
-    <row r="138" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A138" s="4" t="s">
+      <c r="B138" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="B138" s="20" t="s">
-        <v>244</v>
-      </c>
       <c r="C138" s="9"/>
-      <c r="D138" s="19"/>
+      <c r="D138" s="19">
+        <v>3</v>
+      </c>
       <c r="E138" s="20"/>
     </row>
-    <row r="139" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="139" spans="1:5" outlineLevel="1">
       <c r="A139" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B139" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="B139" s="20" t="s">
+      <c r="C139" s="9"/>
+      <c r="D139" s="19">
+        <v>3</v>
+      </c>
+      <c r="E139" s="20"/>
+    </row>
+    <row r="140" spans="1:5" outlineLevel="1">
+      <c r="A140" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B140" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="C139" s="9"/>
-      <c r="D139" s="19"/>
-      <c r="E139" s="20"/>
-    </row>
-    <row r="140" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A140" s="4" t="s">
+      <c r="C140" s="9"/>
+      <c r="D140" s="19">
+        <v>3</v>
+      </c>
+      <c r="E140" s="20"/>
+    </row>
+    <row r="141" spans="1:5" outlineLevel="1">
+      <c r="A141" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B140" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="C140" s="9"/>
-      <c r="D140" s="19"/>
-      <c r="E140" s="20"/>
-    </row>
-    <row r="141" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A141" s="4" t="s">
+      <c r="B141" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="B141" s="20" t="s">
-        <v>240</v>
-      </c>
       <c r="C141" s="9"/>
-      <c r="D141" s="19"/>
+      <c r="D141" s="19">
+        <v>3</v>
+      </c>
       <c r="E141" s="20"/>
     </row>
-    <row r="142" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="142" spans="1:5" outlineLevel="1">
       <c r="A142" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B142" s="20" t="s">
         <v>231</v>
       </c>
-      <c r="B142" s="20" t="s">
+      <c r="C142" s="9"/>
+      <c r="D142" s="19">
+        <v>3</v>
+      </c>
+      <c r="E142" s="20"/>
+    </row>
+    <row r="143" spans="1:5" outlineLevel="1">
+      <c r="A143" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C142" s="9"/>
-      <c r="D142" s="19"/>
-      <c r="E142" s="20"/>
-    </row>
-    <row r="143" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A143" s="4" t="s">
+      <c r="B143" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="B143" s="20" t="s">
-        <v>234</v>
-      </c>
       <c r="C143" s="9"/>
-      <c r="D143" s="19"/>
+      <c r="D143" s="19">
+        <v>3</v>
+      </c>
       <c r="E143" s="20"/>
     </row>
-    <row r="144" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="144" spans="1:5" outlineLevel="1">
       <c r="A144" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B144" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="B144" s="20" t="s">
+      <c r="C144" s="9"/>
+      <c r="D144" s="19">
+        <v>3</v>
+      </c>
+      <c r="E144" s="20"/>
+    </row>
+    <row r="145" spans="1:5" outlineLevel="1">
+      <c r="A145" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="C144" s="9"/>
-      <c r="D144" s="19"/>
-      <c r="E144" s="20"/>
-    </row>
-    <row r="145" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A145" s="4" t="s">
+      <c r="B145" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="B145" s="20" t="s">
+      <c r="C145" s="9"/>
+      <c r="D145" s="19">
+        <v>3</v>
+      </c>
+      <c r="E145" s="20"/>
+    </row>
+    <row r="146" spans="1:5" outlineLevel="1">
+      <c r="A146" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="C145" s="9"/>
-      <c r="D145" s="19"/>
-      <c r="E145" s="20"/>
-    </row>
-    <row r="146" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A146" s="4" t="s">
+      <c r="B146" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B146" s="20" t="s">
-        <v>230</v>
-      </c>
       <c r="C146" s="9"/>
-      <c r="D146" s="19"/>
+      <c r="D146" s="19">
+        <v>3</v>
+      </c>
       <c r="E146" s="20"/>
     </row>
-    <row r="147" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="147" spans="1:5" outlineLevel="1">
       <c r="A147" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B147" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="B147" s="20" t="s">
-        <v>224</v>
-      </c>
       <c r="C147" s="9"/>
-      <c r="D147" s="19"/>
+      <c r="D147" s="19">
+        <v>3</v>
+      </c>
       <c r="E147" s="20"/>
     </row>
-    <row r="148" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="148" spans="1:5" outlineLevel="1">
       <c r="A148" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B148" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="B148" s="20" t="s">
-        <v>222</v>
-      </c>
       <c r="C148" s="9"/>
-      <c r="D148" s="19"/>
+      <c r="D148" s="19">
+        <v>3</v>
+      </c>
       <c r="E148" s="20"/>
     </row>
-    <row r="149" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="149" spans="1:5" outlineLevel="1">
       <c r="A149" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B149" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="B149" s="20" t="s">
-        <v>220</v>
-      </c>
       <c r="C149" s="9"/>
-      <c r="D149" s="19"/>
+      <c r="D149" s="19">
+        <v>3</v>
+      </c>
       <c r="E149" s="20"/>
     </row>
-    <row r="150" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="150" spans="1:5" outlineLevel="1">
       <c r="A150" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B150" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="B150" s="24" t="s">
-        <v>218</v>
-      </c>
       <c r="C150" s="9"/>
-      <c r="D150" s="19"/>
+      <c r="D150" s="19">
+        <v>3</v>
+      </c>
       <c r="E150" s="20"/>
     </row>
-    <row r="151" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="151" spans="1:5" outlineLevel="1">
       <c r="A151" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B151" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="B151" s="24" t="s">
-        <v>216</v>
-      </c>
       <c r="C151" s="9"/>
-      <c r="D151" s="19"/>
+      <c r="D151" s="19">
+        <v>3</v>
+      </c>
       <c r="E151" s="20"/>
     </row>
-    <row r="152" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="152" spans="1:5" outlineLevel="1">
       <c r="A152" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B152" t="s">
+        <v>210</v>
+      </c>
+      <c r="D152" s="19">
+        <v>1</v>
+      </c>
+      <c r="E152" s="20"/>
+    </row>
+    <row r="153" spans="1:5" outlineLevel="1">
+      <c r="A153" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B152" t="s">
-        <v>211</v>
-      </c>
-      <c r="D152" s="19">
-        <v>1</v>
-      </c>
-      <c r="E152" s="20"/>
-    </row>
-    <row r="153" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A153" s="4" t="s">
+      <c r="B153" t="s">
         <v>213</v>
       </c>
-      <c r="B153" t="s">
-        <v>214</v>
-      </c>
-      <c r="D153" s="19"/>
+      <c r="D153" s="19">
+        <v>1</v>
+      </c>
       <c r="E153" s="20">
         <f>165-96</f>
         <v>69</v>
       </c>
     </row>
-    <row r="154" spans="1:5" collapsed="1">
+    <row r="154" spans="1:5">
       <c r="A154" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B154" s="20" t="s">
         <v>118</v>
-      </c>
-      <c r="B154" s="20" t="s">
-        <v>119</v>
       </c>
       <c r="C154" s="9"/>
       <c r="D154" s="19">
@@ -3418,261 +3632,414 @@
       </c>
       <c r="E154" s="20"/>
     </row>
-    <row r="155" spans="1:5" hidden="1" outlineLevel="1">
+    <row r="155" spans="1:5" outlineLevel="1">
       <c r="A155" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B155" t="s">
         <v>53</v>
       </c>
-      <c r="B155" t="s">
+      <c r="D155" s="19">
+        <v>1</v>
+      </c>
+      <c r="E155" s="20"/>
+    </row>
+    <row r="156" spans="1:5" outlineLevel="1">
+      <c r="A156" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D155" s="19">
-        <v>1</v>
-      </c>
-      <c r="E155" s="20"/>
-    </row>
-    <row r="156" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A156" s="7" t="s">
+      <c r="B156" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="D156" s="19">
+        <v>1</v>
+      </c>
+      <c r="E156" s="20"/>
+    </row>
+    <row r="157" spans="1:5" outlineLevel="1">
+      <c r="A157" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D156" s="19">
-        <v>1</v>
-      </c>
-      <c r="E156" s="20"/>
-    </row>
-    <row r="157" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A157" s="4" t="s">
+      <c r="B157" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="D157" s="19">
+        <v>1</v>
+      </c>
+      <c r="E157" s="20"/>
+    </row>
+    <row r="158" spans="1:5" outlineLevel="1">
+      <c r="A158" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D157" s="19">
-        <v>1</v>
-      </c>
-      <c r="E157" s="20"/>
-    </row>
-    <row r="158" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A158" s="4" t="s">
+      <c r="B158" t="s">
         <v>59</v>
       </c>
-      <c r="B158" t="s">
+      <c r="D158" s="19">
+        <v>1</v>
+      </c>
+      <c r="E158" s="20"/>
+    </row>
+    <row r="159" spans="1:5" outlineLevel="1">
+      <c r="A159" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D158" s="19">
-        <v>1</v>
-      </c>
-      <c r="E158" s="20"/>
-    </row>
-    <row r="159" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A159" s="4" t="s">
+      <c r="B159" t="s">
         <v>61</v>
       </c>
-      <c r="B159" t="s">
+      <c r="D159" s="19">
+        <v>1</v>
+      </c>
+      <c r="E159" s="20"/>
+    </row>
+    <row r="160" spans="1:5" outlineLevel="1">
+      <c r="A160" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D159" s="19">
-        <v>1</v>
-      </c>
-      <c r="E159" s="20"/>
-    </row>
-    <row r="160" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A160" s="4" t="s">
+      <c r="B160" t="s">
         <v>63</v>
       </c>
-      <c r="B160" t="s">
+      <c r="D160" s="19">
+        <v>1</v>
+      </c>
+      <c r="E160" s="20"/>
+    </row>
+    <row r="161" spans="1:5" outlineLevel="1">
+      <c r="A161" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D160" s="19">
-        <v>1</v>
-      </c>
-      <c r="E160" s="20"/>
-    </row>
-    <row r="161" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A161" s="4" t="s">
+      <c r="B161" t="s">
         <v>65</v>
       </c>
-      <c r="B161" t="s">
+      <c r="D161" s="19">
+        <v>1</v>
+      </c>
+      <c r="E161" s="20"/>
+    </row>
+    <row r="162" spans="1:5" outlineLevel="1">
+      <c r="A162" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D161" s="19">
-        <v>1</v>
-      </c>
-      <c r="E161" s="20"/>
-    </row>
-    <row r="162" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A162" s="7" t="s">
+      <c r="B162" t="s">
         <v>67</v>
       </c>
-      <c r="B162" t="s">
+      <c r="D162" s="19">
+        <v>1</v>
+      </c>
+      <c r="E162" s="20"/>
+    </row>
+    <row r="163" spans="1:5" outlineLevel="1">
+      <c r="A163" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D162" s="19">
-        <v>1</v>
-      </c>
-      <c r="E162" s="20"/>
-    </row>
-    <row r="163" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A163" s="7" t="s">
+      <c r="B163" t="s">
         <v>69</v>
       </c>
-      <c r="B163" t="s">
+      <c r="D163" s="19">
+        <v>1</v>
+      </c>
+      <c r="E163" s="20"/>
+    </row>
+    <row r="164" spans="1:5" outlineLevel="1">
+      <c r="A164" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D163" s="19">
-        <v>1</v>
-      </c>
-      <c r="E163" s="20"/>
-    </row>
-    <row r="164" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A164" s="4" t="s">
+      <c r="B164" t="s">
         <v>71</v>
       </c>
-      <c r="B164" t="s">
+      <c r="D164" s="19">
+        <v>1</v>
+      </c>
+      <c r="E164" s="20"/>
+    </row>
+    <row r="165" spans="1:5" outlineLevel="1">
+      <c r="A165" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D164" s="19">
-        <v>1</v>
-      </c>
-      <c r="E164" s="20"/>
-    </row>
-    <row r="165" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A165" s="1" t="s">
+      <c r="D165" s="19">
+        <v>4</v>
+      </c>
+      <c r="E165" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="D165" s="19">
-        <v>3</v>
-      </c>
-      <c r="E165" s="20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" collapsed="1">
+    </row>
+    <row r="166" spans="1:5">
       <c r="A166" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B166" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C166" s="9"/>
       <c r="D166" s="19">
         <v>3</v>
       </c>
-      <c r="E166" s="20"/>
-    </row>
-    <row r="167" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="E166" s="22"/>
+    </row>
+    <row r="167" spans="1:5" outlineLevel="1">
       <c r="C167"/>
       <c r="D167" s="20"/>
-      <c r="E167" s="20"/>
-    </row>
-    <row r="168" spans="1:5" collapsed="1">
+      <c r="E167" s="22"/>
+    </row>
+    <row r="168" spans="1:5">
       <c r="A168" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B168" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C168" s="9"/>
       <c r="D168" s="19">
         <v>3</v>
       </c>
-      <c r="E168" s="20"/>
-    </row>
-    <row r="169" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="E168" s="22"/>
+    </row>
+    <row r="169" spans="1:5" outlineLevel="1">
       <c r="D169" s="19"/>
-      <c r="E169" s="20"/>
-    </row>
-    <row r="170" spans="1:5" collapsed="1">
+      <c r="E169" s="22"/>
+    </row>
+    <row r="170" spans="1:5">
       <c r="A170" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B170" s="20" t="s">
         <v>104</v>
-      </c>
-      <c r="B170" s="20" t="s">
-        <v>105</v>
       </c>
       <c r="C170" s="9"/>
       <c r="D170" s="19">
         <v>3</v>
       </c>
-      <c r="E170" s="20"/>
-    </row>
-    <row r="171" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="E170" s="22"/>
+    </row>
+    <row r="171" spans="1:5" outlineLevel="1">
       <c r="D171" s="19"/>
-      <c r="E171" s="20"/>
-    </row>
-    <row r="172" spans="1:5" collapsed="1">
+      <c r="E171" s="22"/>
+    </row>
+    <row r="172" spans="1:5">
       <c r="A172" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B172" s="20" t="s">
         <v>120</v>
-      </c>
-      <c r="B172" s="20" t="s">
-        <v>121</v>
       </c>
       <c r="C172" s="9"/>
       <c r="D172" s="19">
         <v>3</v>
       </c>
-      <c r="E172" s="20"/>
-    </row>
-    <row r="173" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="E172" s="22"/>
+    </row>
+    <row r="173" spans="1:5" outlineLevel="1">
       <c r="A173" s="11"/>
       <c r="B173" s="11"/>
       <c r="C173" s="12"/>
       <c r="D173" s="23"/>
       <c r="E173" s="22"/>
     </row>
-    <row r="174" spans="1:5" collapsed="1">
+    <row r="174" spans="1:5">
       <c r="A174" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B174" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="B174" s="20" t="s">
-        <v>123</v>
       </c>
       <c r="C174" s="9"/>
       <c r="D174" s="19">
         <v>3</v>
       </c>
-      <c r="E174" s="20"/>
-    </row>
-    <row r="175" spans="1:5" hidden="1" outlineLevel="1">
+      <c r="E174" s="22"/>
+    </row>
+    <row r="175" spans="1:5" outlineLevel="1">
       <c r="A175" s="11"/>
       <c r="B175" s="11"/>
       <c r="C175" s="12"/>
       <c r="D175" s="23"/>
       <c r="E175" s="22"/>
     </row>
-    <row r="176" spans="1:5" collapsed="1">
+    <row r="176" spans="1:5">
       <c r="A176" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B176" s="20" t="s">
         <v>124</v>
-      </c>
-      <c r="B176" s="20" t="s">
-        <v>125</v>
       </c>
       <c r="C176" s="9"/>
       <c r="D176" s="19">
         <v>3</v>
       </c>
-      <c r="E176" s="20"/>
-    </row>
-    <row r="177" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A177" s="11"/>
-      <c r="B177" s="11"/>
+      <c r="E176" s="22"/>
+    </row>
+    <row r="177" spans="1:5" outlineLevel="1">
+      <c r="A177" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="B177" s="11" t="s">
+        <v>350</v>
+      </c>
       <c r="C177" s="12"/>
-      <c r="D177" s="23"/>
+      <c r="D177" s="23">
+        <v>1</v>
+      </c>
       <c r="E177" s="22"/>
     </row>
-    <row r="178" spans="1:5" collapsed="1">
-      <c r="A178" s="14" t="s">
-        <v>206</v>
+    <row r="178" spans="1:5" outlineLevel="1">
+      <c r="A178" s="18" t="s">
+        <v>351</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>207</v>
+        <v>352</v>
       </c>
       <c r="C178" s="12"/>
       <c r="D178" s="23">
-        <v>3</v>
-      </c>
-      <c r="E178" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="E178" s="22"/>
+    </row>
+    <row r="179" spans="1:5" outlineLevel="1">
+      <c r="A179" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="B179" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="C179" s="12"/>
+      <c r="D179" s="23">
+        <v>1</v>
+      </c>
+      <c r="E179" s="22"/>
+    </row>
+    <row r="180" spans="1:5" outlineLevel="1">
+      <c r="A180" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="B180" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="C180" s="12"/>
+      <c r="D180" s="23">
+        <v>1</v>
+      </c>
+      <c r="E180" s="22"/>
+    </row>
+    <row r="181" spans="1:5" outlineLevel="1">
+      <c r="A181" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="B181" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="C181" s="12"/>
+      <c r="D181" s="23">
+        <v>1</v>
+      </c>
+      <c r="E181" s="22"/>
+    </row>
+    <row r="182" spans="1:5" outlineLevel="1">
+      <c r="A182" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="B182" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="C182" s="12"/>
+      <c r="D182" s="23">
+        <v>1</v>
+      </c>
+      <c r="E182" s="22"/>
+    </row>
+    <row r="183" spans="1:5" outlineLevel="1">
+      <c r="A183" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="B183" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="C183" s="12"/>
+      <c r="D183" s="23">
+        <v>4</v>
+      </c>
+      <c r="E183" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" outlineLevel="1">
+      <c r="A184" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="B184" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="C184" s="12"/>
+      <c r="D184" s="23">
+        <v>2</v>
+      </c>
+      <c r="E184" s="22"/>
+    </row>
+    <row r="185" spans="1:5" outlineLevel="1">
+      <c r="A185" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="B185" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="C185" s="12"/>
+      <c r="D185" s="23">
+        <v>2</v>
+      </c>
+      <c r="E185" s="22"/>
+    </row>
+    <row r="186" spans="1:5" outlineLevel="1">
+      <c r="A186" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="B186" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="C186" s="12"/>
+      <c r="D186" s="23">
+        <v>3</v>
+      </c>
+      <c r="E186" s="22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="B187" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C187" s="12"/>
+      <c r="D187" s="23">
+        <v>1</v>
+      </c>
+      <c r="E187" s="20"/>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2">
+      <c r="B209">
+        <f>3+5+3+4+2+3</f>
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3770,7 +4137,7 @@
     <hyperlink ref="A53" r:id="rId92" location="GET_search.2Fparser"/>
     <hyperlink ref="A54" r:id="rId93" location="GET_search.2Ftimeparser"/>
     <hyperlink ref="A55" r:id="rId94" location="search.2Ftypeahead"/>
-    <hyperlink ref="A178" r:id="rId95"/>
+    <hyperlink ref="A187" r:id="rId95"/>
     <hyperlink ref="A166" r:id="rId96"/>
     <hyperlink ref="A152" r:id="rId97" location="POST_receivers.2Fsimple"/>
     <hyperlink ref="A151" r:id="rId98" location="GET_indexing.2Fpreview.2F.7Bjob_id.7D"/>
@@ -3842,11 +4209,20 @@
     <hyperlink ref="A89" r:id="rId164" location="POST_data.2Finputs.2Fad.2F.7Bname.7D"/>
     <hyperlink ref="A85" r:id="rId165" location="GET_data.2Finputs.2Fad"/>
     <hyperlink ref="A86" r:id="rId166" location="POST_data.2Finputs.2Fad"/>
+    <hyperlink ref="A177" r:id="rId167" location="GET_messages"/>
+    <hyperlink ref="A178" r:id="rId168"/>
+    <hyperlink ref="A179" r:id="rId169" location="DELETE_messages.2F.7Bname.7D"/>
+    <hyperlink ref="A180" r:id="rId170" location="GET_server.2Fcontrol"/>
+    <hyperlink ref="A181" r:id="rId171" location="POST_server.2Fcontrol.2Frestart"/>
+    <hyperlink ref="A182" r:id="rId172" location="GET_server.2Finfo"/>
+    <hyperlink ref="A184" r:id="rId173" location="GET_server.2Flogger"/>
+    <hyperlink ref="A185" r:id="rId174" location="GET_server.2Flogger.2F.7Bname.7D"/>
+    <hyperlink ref="A186" r:id="rId175" location="POST_server.2Flogger.2F.7Bname.7D"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
-    <tablePart r:id="rId167"/>
+    <tablePart r:id="rId176"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>